<commit_message>
Frontend: Redux, FetchAPI, Chart.js, Excel.js Created and Completed
</commit_message>
<xml_diff>
--- a/backend/public/temp/Employee Data.xlsx
+++ b/backend/public/temp/Employee Data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FE6FBC4-A7BA-4014-A39C-2206E3FCCB44}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{281CCE29-B102-4CBB-BB80-A5E66C9F2263}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>employeeID</t>
   </si>
@@ -72,46 +72,7 @@
     <t>present</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF49E9A6"/>
-        <rFont val="Consolas"/>
-      </rPr>
-      <t>JavaScript</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBECFDA"/>
-        <rFont val="Consolas"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF49E9A6"/>
-        <rFont val="Consolas"/>
-      </rPr>
-      <t>React</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBECFDA"/>
-        <rFont val="Consolas"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF49E9A6"/>
-        <rFont val="Consolas"/>
-      </rPr>
-      <t>Node.js, Express.js</t>
-    </r>
+    <t>JavaScript, React, Node.js, Express.js</t>
   </si>
   <si>
     <t>John</t>
@@ -127,6 +88,63 @@
   </si>
   <si>
     <t>Jatin</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>React, JavaScript, Node.js, Express.js, MongoDB</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Sr. Java Developer</t>
+  </si>
+  <si>
+    <t>Java, Spring Boot, Hibernate</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Sr. .NET Developer</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>C#, .NET, SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David      </t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Jr. Front-end Developer</t>
+  </si>
+  <si>
+    <t>JavaScript, front end Development, react</t>
+  </si>
+  <si>
+    <t>Mehul</t>
   </si>
 </sst>
 </file>
@@ -149,19 +167,20 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF7060EB"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF49E9A6"/>
+      <color theme="1"/>
       <name val="Consolas"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFBECFDA"/>
-      <name val="Consolas"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Söhne Mono"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,13 +203,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,7 +539,7 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -525,91 +547,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>43101</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>35849</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>80000</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>44927</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>37761</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <v>30000</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7">
+        <v>45025</v>
+      </c>
+      <c r="F4" s="7">
+        <v>37760</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="6">
+        <v>34980</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7">
+        <v>44012</v>
+      </c>
+      <c r="F5" s="7">
+        <v>34926</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45000</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7">
+        <v>40226</v>
+      </c>
+      <c r="F6" s="7">
+        <v>33936</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="6">
+        <v>62000</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7">
+        <v>44842</v>
+      </c>
+      <c r="F7" s="7">
+        <v>36943</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="6">
+        <v>20000</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75">
+      <c r="A15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>